<commit_message>
51020: update Project> Timesheet detail: Add button Export TS Detail [BE]
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/TSDetail.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/TSDetail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ncc-erp-project\aspnet-core\src\ProjectManagement.Web.Host\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2F2AE2-41E5-4760-9768-BD79E9471ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFEA589-DAAF-46E6-B1B4-6BD4BB98AE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,7 +326,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -450,9 +450,6 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -492,17 +489,17 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1038,10 +1035,10 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:H24"/>
+  <dimension ref="B1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="E7" sqref="E7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.8"/>
@@ -1057,8 +1054,8 @@
     <col min="10" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="27" customHeight="1"/>
-    <row r="2" spans="2:7" ht="43.5" customHeight="1" thickBot="1">
+    <row r="1" spans="2:9" ht="27" customHeight="1"/>
+    <row r="2" spans="2:9" ht="43.5" customHeight="1" thickBot="1">
       <c r="B2" s="28"/>
       <c r="C2" s="39"/>
       <c r="D2" s="28"/>
@@ -1066,71 +1063,73 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="2:7" ht="24" customHeight="1" thickTop="1">
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+    <row r="3" spans="2:9" ht="24" customHeight="1" thickTop="1">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="40"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="2:7" ht="24" customHeight="1">
+      <c r="F3" s="45"/>
+      <c r="G3" s="43"/>
+    </row>
+    <row r="4" spans="2:9" ht="24" customHeight="1">
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="45"/>
-    </row>
-    <row r="6" spans="2:7" ht="24.6">
-      <c r="B6" s="55" t="s">
+      <c r="F4" s="46"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="6" spans="2:9" ht="24.6">
+      <c r="B6" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="56"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-    </row>
-    <row r="10" spans="2:7" ht="12.75" customHeight="1">
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="2:9" ht="12.75" customHeight="1">
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
       <c r="E10"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="2:7" ht="6.75" customHeight="1">
+    <row r="11" spans="2:9" ht="6.75" customHeight="1">
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
       <c r="E11"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" ht="6" customHeight="1" thickBot="1">
+    <row r="12" spans="2:9" ht="6" customHeight="1" thickBot="1">
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
@@ -1138,13 +1137,13 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="2:7" ht="14.4" thickTop="1">
+    <row r="13" spans="2:9" ht="14.4" thickTop="1">
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:9">
       <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="18.75" customHeight="1">
+    <row r="15" spans="2:9" ht="18.75" customHeight="1">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="19"/>
@@ -1172,7 +1171,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:7" ht="18" customHeight="1">
+    <row r="16" spans="2:9" ht="18" customHeight="1">
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -1201,16 +1200,16 @@
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="50"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" thickBot="1">
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="51"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="2:8" ht="14.4" thickTop="1"/>
     <row r="22" spans="2:8">
@@ -1230,18 +1229,17 @@
       <c r="G23" s="17"/>
     </row>
     <row r="24" spans="2:8" ht="27" customHeight="1">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="18"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="12">
-    <mergeCell ref="E6:G6"/>
+  <mergeCells count="11">
     <mergeCell ref="E7:G9"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="G3:G4"/>
@@ -1252,7 +1250,7 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1281,12 +1279,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26.4">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="2:6" ht="13.8">
       <c r="B3" s="2" t="s">
@@ -1311,10 +1309,10 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="2:6" ht="10.8" thickBot="1">
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="10.8" thickTop="1"/>
   </sheetData>

</xml_diff>